<commit_message>
UI Visibility toggles setup
</commit_message>
<xml_diff>
--- a/DesignDoc/CardLibrary.xlsx
+++ b/DesignDoc/CardLibrary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unreal Projects\SiegeTactics\SiegeTactics\DesignDoc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unreal Projects\SiegeTactics\AutoSiege\DesignDoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B317ABE-1374-4343-B45B-78CE4EB33EA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC0175A-254D-48A5-85F2-DF209C3D9C43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38010" yWindow="390" windowWidth="28800" windowHeight="15555" xr2:uid="{FFD96320-E16A-4A22-8FE4-AD96CB7CA0C5}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{FFD96320-E16A-4A22-8FE4-AD96CB7CA0C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,12 +22,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -583,24 +577,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -615,10 +597,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -933,16 +914,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893417B8-0E04-4E14-A7DD-266D70EB268C}">
-  <dimension ref="A1:H85"/>
+  <dimension ref="A1:H84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" customWidth="1"/>
-    <col min="5" max="5" width="69.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" style="1" customWidth="1"/>
+    <col min="2" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="69.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -978,7 +961,6 @@
       <c r="B2" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C2" s="1"/>
       <c r="D2" s="1">
         <v>1</v>
       </c>
@@ -1002,7 +984,6 @@
       <c r="B3" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C3" s="1"/>
       <c r="D3" s="1">
         <v>1</v>
       </c>
@@ -1026,7 +1007,6 @@
       <c r="B4" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C4" s="1"/>
       <c r="D4" s="1">
         <v>1</v>
       </c>
@@ -1043,7 +1023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1066,7 +1046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -1089,7 +1069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1112,7 +1092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1135,7 +1115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1158,7 +1138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -1181,7 +1161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -1204,7 +1184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1227,7 +1207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -1250,7 +1230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
@@ -1273,7 +1253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
@@ -1296,7 +1276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -1319,7 +1299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
@@ -1342,7 +1322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>39</v>
       </c>
@@ -1365,7 +1345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -1388,7 +1368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>43</v>
       </c>
@@ -1411,7 +1391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>45</v>
       </c>
@@ -1434,7 +1414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>47</v>
       </c>
@@ -1457,7 +1437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>49</v>
       </c>
@@ -1480,7 +1460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>51</v>
       </c>
@@ -1503,7 +1483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
@@ -1526,7 +1506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>56</v>
       </c>
@@ -1549,7 +1529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>57</v>
       </c>
@@ -1572,7 +1552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>59</v>
       </c>
@@ -1595,7 +1575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>61</v>
       </c>
@@ -1618,7 +1598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>63</v>
       </c>
@@ -1641,7 +1621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>65</v>
       </c>
@@ -1664,7 +1644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>67</v>
       </c>
@@ -1687,7 +1667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>69</v>
       </c>
@@ -1710,7 +1690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>71</v>
       </c>
@@ -1733,7 +1713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>73</v>
       </c>
@@ -1756,7 +1736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>75</v>
       </c>
@@ -1779,7 +1759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>77</v>
       </c>
@@ -1802,7 +1782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>79</v>
       </c>
@@ -1825,7 +1805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>81</v>
       </c>
@@ -1848,7 +1828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>83</v>
       </c>
@@ -1871,7 +1851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>85</v>
       </c>
@@ -1894,7 +1874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>87</v>
       </c>
@@ -1917,7 +1897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>88</v>
       </c>
@@ -1940,7 +1920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>90</v>
       </c>
@@ -1963,7 +1943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>92</v>
       </c>
@@ -1986,7 +1966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>94</v>
       </c>
@@ -2009,7 +1989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>96</v>
       </c>
@@ -2032,7 +2012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>98</v>
       </c>
@@ -2055,7 +2035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>100</v>
       </c>
@@ -2078,7 +2058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>102</v>
       </c>
@@ -2101,7 +2081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>104</v>
       </c>
@@ -2124,7 +2104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>106</v>
       </c>
@@ -2147,7 +2127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>108</v>
       </c>
@@ -2170,7 +2150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>110</v>
       </c>
@@ -2193,7 +2173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>112</v>
       </c>
@@ -2216,7 +2196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>114</v>
       </c>
@@ -2239,7 +2219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>116</v>
       </c>
@@ -2262,7 +2242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>118</v>
       </c>
@@ -2285,7 +2265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>120</v>
       </c>
@@ -2308,7 +2288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>122</v>
       </c>
@@ -2331,7 +2311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>124</v>
       </c>
@@ -2354,7 +2334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>126</v>
       </c>
@@ -2377,7 +2357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>128</v>
       </c>
@@ -2400,7 +2380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>130</v>
       </c>
@@ -2423,7 +2403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>132</v>
       </c>
@@ -2446,7 +2426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>134</v>
       </c>
@@ -2469,7 +2449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>136</v>
       </c>
@@ -2492,7 +2472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>138</v>
       </c>
@@ -2516,398 +2496,372 @@
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+      <c r="A69" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B69" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2">
+      <c r="D69" s="1">
         <v>5</v>
       </c>
-      <c r="E69" s="2" t="s">
+      <c r="E69" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F69" s="2">
-        <v>2</v>
-      </c>
-      <c r="G69" s="2">
-        <v>2</v>
-      </c>
-      <c r="H69" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
+      <c r="F69" s="1">
+        <v>2</v>
+      </c>
+      <c r="G69" s="1">
+        <v>2</v>
+      </c>
+      <c r="H69" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B70" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2">
+      <c r="D70" s="1">
         <v>5</v>
       </c>
-      <c r="E70" s="2" t="s">
+      <c r="E70" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="F70" s="2">
+      <c r="F70" s="1">
         <v>9</v>
       </c>
-      <c r="G70" s="2">
+      <c r="G70" s="1">
         <v>7</v>
       </c>
-      <c r="H70" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
+      <c r="H70" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B71" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2">
+      <c r="D71" s="1">
         <v>5</v>
       </c>
-      <c r="E71" s="2" t="s">
+      <c r="E71" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F71" s="2">
+      <c r="F71" s="1">
         <v>0</v>
       </c>
-      <c r="G71" s="2">
+      <c r="G71" s="1">
         <v>5</v>
       </c>
-      <c r="H71" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
+      <c r="H71" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B72" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2">
+      <c r="D72" s="1">
         <v>5</v>
       </c>
-      <c r="E72" s="2" t="s">
+      <c r="E72" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="F72" s="2">
+      <c r="F72" s="1">
         <v>5</v>
       </c>
-      <c r="G72" s="2">
+      <c r="G72" s="1">
         <v>7</v>
       </c>
-      <c r="H72" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
+      <c r="H72" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B73" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2">
+      <c r="D73" s="1">
         <v>5</v>
       </c>
-      <c r="E73" s="2" t="s">
+      <c r="E73" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F73" s="2">
+      <c r="F73" s="1">
         <v>6</v>
       </c>
-      <c r="G73" s="2">
+      <c r="G73" s="1">
         <v>5</v>
       </c>
-      <c r="H73" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
+      <c r="H73" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B74" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2">
+      <c r="D74" s="1">
         <v>5</v>
       </c>
-      <c r="E74" s="2" t="s">
+      <c r="E74" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F74" s="2">
-        <v>2</v>
-      </c>
-      <c r="G74" s="2">
-        <v>3</v>
-      </c>
-      <c r="H74" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
+      <c r="F74" s="1">
+        <v>2</v>
+      </c>
+      <c r="G74" s="1">
+        <v>3</v>
+      </c>
+      <c r="H74" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B75" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C75" s="2"/>
-      <c r="D75" s="2">
+      <c r="D75" s="1">
         <v>5</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="E75" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="F75" s="2">
+      <c r="F75" s="1">
         <v>6</v>
       </c>
-      <c r="G75" s="2">
+      <c r="G75" s="1">
         <v>7</v>
       </c>
-      <c r="H75" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
+      <c r="H75" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B76" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2">
+      <c r="D76" s="1">
         <v>5</v>
       </c>
-      <c r="E76" s="2" t="s">
+      <c r="E76" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="F76" s="2">
-        <v>3</v>
-      </c>
-      <c r="G76" s="2">
+      <c r="F76" s="1">
+        <v>3</v>
+      </c>
+      <c r="G76" s="1">
         <v>9</v>
       </c>
-      <c r="H76" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
+      <c r="H76" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B77" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C77" s="2"/>
-      <c r="D77" s="2">
+      <c r="D77" s="1">
         <v>6</v>
       </c>
-      <c r="E77" s="2" t="s">
+      <c r="E77" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F77" s="2">
+      <c r="F77" s="1">
         <v>6</v>
       </c>
-      <c r="G77" s="2">
+      <c r="G77" s="1">
         <v>9</v>
       </c>
-      <c r="H77" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
+      <c r="H77" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B78" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C78" s="2"/>
-      <c r="D78" s="2">
+      <c r="D78" s="1">
         <v>6</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="E78" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F78" s="2">
+      <c r="F78" s="1">
         <v>5</v>
       </c>
-      <c r="G78" s="2">
-        <v>4</v>
-      </c>
-      <c r="H78" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
+      <c r="G78" s="1">
+        <v>4</v>
+      </c>
+      <c r="H78" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B79" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2">
+      <c r="D79" s="1">
         <v>6</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="E79" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F79" s="2">
+      <c r="F79" s="1">
         <v>7</v>
       </c>
-      <c r="G79" s="2">
+      <c r="G79" s="1">
         <v>7</v>
       </c>
-      <c r="H79" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
+      <c r="H79" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B80" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2">
+      <c r="D80" s="1">
         <v>6</v>
       </c>
-      <c r="E80" s="2" t="s">
+      <c r="E80" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="F80" s="2">
-        <v>3</v>
-      </c>
-      <c r="G80" s="2">
+      <c r="F80" s="1">
+        <v>3</v>
+      </c>
+      <c r="G80" s="1">
         <v>6</v>
       </c>
-      <c r="H80" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
+      <c r="H80" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B81" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C81" s="2"/>
-      <c r="D81" s="2">
+      <c r="D81" s="1">
         <v>6</v>
       </c>
-      <c r="E81" s="2" t="s">
+      <c r="E81" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F81" s="2">
-        <v>2</v>
-      </c>
-      <c r="G81" s="2">
+      <c r="F81" s="1">
+        <v>2</v>
+      </c>
+      <c r="G81" s="1">
         <v>8</v>
       </c>
-      <c r="H81" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
+      <c r="H81" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B82" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C82" s="2"/>
-      <c r="D82" s="2">
+      <c r="D82" s="1">
         <v>6</v>
       </c>
-      <c r="E82" s="2" t="s">
+      <c r="E82" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="F82" s="2">
-        <v>4</v>
-      </c>
-      <c r="G82" s="2">
-        <v>4</v>
-      </c>
-      <c r="H82" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
+      <c r="F82" s="1">
+        <v>4</v>
+      </c>
+      <c r="G82" s="1">
+        <v>4</v>
+      </c>
+      <c r="H82" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B83" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C83" s="2"/>
-      <c r="D83" s="2">
+      <c r="D83" s="1">
         <v>6</v>
       </c>
-      <c r="E83" s="2" t="s">
+      <c r="E83" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="F83" s="2">
+      <c r="F83" s="1">
         <v>5</v>
       </c>
-      <c r="G83" s="2">
+      <c r="G83" s="1">
         <v>7</v>
       </c>
-      <c r="H83" s="2">
+      <c r="H83" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
+      <c r="A84" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B84" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C84" s="2"/>
-      <c r="D84" s="2">
+      <c r="D84" s="1">
         <v>6</v>
       </c>
-      <c r="E84" s="2" t="s">
+      <c r="E84" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="F84" s="2">
+      <c r="F84" s="1">
         <v>7</v>
       </c>
-      <c r="G84" s="2">
+      <c r="G84" s="1">
         <v>10</v>
       </c>
-      <c r="H84" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="2"/>
-      <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="2"/>
-      <c r="E85" s="2"/>
-      <c r="F85" s="2"/>
-      <c r="G85" s="2"/>
-      <c r="H85" s="2"/>
+      <c r="H84" s="1">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H84" xr:uid="{104CD0FF-1B12-42B8-9BF6-324AEB9FF83D}"/>

</xml_diff>